<commit_message>
Sync with Latest changes
</commit_message>
<xml_diff>
--- a/Code/HA-Models/Target_AggMPCX_LiquWealth/Data_AggMPC_LotteryWin.xlsx
+++ b/Code/HA-Models/Target_AggMPCX_LiquWealth/Data_AggMPC_LotteryWin.xlsx
@@ -405,7 +405,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.5047414390501345</v>
+        <v>0.5033237371360078</v>
       </c>
       <c r="D2">
         <v>0.5056845</v>
@@ -419,7 +419,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.1779497140893118</v>
+        <v>0.1780008224915589</v>
       </c>
       <c r="D3">
         <v>0.1759051</v>
@@ -433,7 +433,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.09026214638458505</v>
+        <v>0.09040054955377354</v>
       </c>
       <c r="D4">
         <v>0.1035106</v>
@@ -447,7 +447,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.04992188069439409</v>
+        <v>0.05002666149093139</v>
       </c>
       <c r="D5">
         <v>0.0444222</v>
@@ -461,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.03012443836764029</v>
+        <v>0.03022457184546027</v>
       </c>
       <c r="D6">
         <v>0.0336616</v>

</xml_diff>